<commit_message>
Support LINK price feed from USD to wei
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lancewhatley/moontography/contracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5DBCD8-3719-2842-A961-D934432F07F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C19E22-9C38-EC4B-87A1-51DB2B2AE7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{B57A1663-67F0-A447-9066-7726D1B320E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -815,39 +815,39 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <f>$C9/D2</f>
-        <v>0</v>
+        <v>4.5454545454545455E-4</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:J9" si="6">$C9/E2</f>
-        <v>0</v>
+        <v>3.3333333333333335E-3</v>
       </c>
       <c r="F9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>9.1407678244972576E-2</v>
       </c>
       <c r="H9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="I9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.2658227848101264</v>
       </c>
       <c r="J9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.3137436372049978E-2</v>
       </c>
       <c r="K9">
         <f>$C9/K2</f>
-        <v>0</v>
+        <v>4.5454545454545455E-4</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add buyback util contract
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lancewhatley/moontography/contracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C19E22-9C38-EC4B-87A1-51DB2B2AE7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9072D44A-46A0-844D-BE8B-79F22F9967E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{B57A1663-67F0-A447-9066-7726D1B320E6}"/>
   </bookViews>
@@ -815,39 +815,39 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <f>$C9/D2</f>
-        <v>4.5454545454545455E-4</v>
+        <v>1.1363636363636363E-3</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:J9" si="6">$C9/E2</f>
-        <v>3.3333333333333335E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="F9">
         <f t="shared" si="6"/>
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <f t="shared" si="6"/>
-        <v>9.1407678244972576E-2</v>
+        <v>0.22851919561243145</v>
       </c>
       <c r="H9">
         <f t="shared" si="6"/>
-        <v>2.2222222222222223E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="I9">
         <f t="shared" si="6"/>
-        <v>1.2658227848101264</v>
+        <v>3.1645569620253164</v>
       </c>
       <c r="J9">
         <f t="shared" si="6"/>
-        <v>2.3137436372049978E-2</v>
+        <v>5.7843590930124943E-2</v>
       </c>
       <c r="K9">
         <f>$C9/K2</f>
-        <v>4.5454545454545455E-4</v>
+        <v>1.1363636363636363E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>